<commit_message>
Fixed PPB reading only from sheet 2
</commit_message>
<xml_diff>
--- a/working/CyprotexFup/EPA_PPB_09032020_Summary_Result_Final.xlsx
+++ b/working/CyprotexFup/EPA_PPB_09032020_Summary_Result_Final.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\CLIENT_DATA\EPA\EPA 2020\Reporting\September 2020\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwambaug\git\invitroTKstats\working\CyprotexFup\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A918B0A8-0E64-4F4F-9C15-0084D02DEC52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="3720" yWindow="3720" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="3" r:id="rId1"/>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="925" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="925" uniqueCount="234">
   <si>
     <t>SampleName</t>
   </si>
@@ -392,27 +393,6 @@
   </si>
   <si>
     <t xml:space="preserve">DTXSID5021758-30_Human_Plasma_T0_2_____xP1-_Inj 72  </t>
-  </si>
-  <si>
-    <t>DTXSID3024621-30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DTXSID3024621-30_Human_PBS__1_____xP1-_Inj 127  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">DTXSID3024621-30_Human_PBS__2_____xP1-_Inj 128  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">DTXSID3024621-30_Human_Plasma__1_____xP1-_Inj 129  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">DTXSID3024621-30_Human_Plasma__2_____xP1-_Inj 130  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">DTXSID3024621-30_Human_Plasma_T0_1_____xP1-_Inj 131  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">DTXSID3024621-30_Human_Plasma_T0_2_____xP1-_Inj 132  </t>
   </si>
   <si>
     <t>DTXSID6021032-30</t>
@@ -744,9 +724,6 @@
     <t>DTXSID6021032</t>
   </si>
   <si>
-    <t>DTXSID3024621</t>
-  </si>
-  <si>
     <t>Plasma Protein Binding: Data Summary</t>
   </si>
   <si>
@@ -760,12 +737,33 @@
   </si>
   <si>
     <t>&lt; 1%</t>
+  </si>
+  <si>
+    <t>DTXSID1024621-30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DTXSID1024621-30_Human_Plasma__1_____xP1-_Inj 129  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DTXSID1024621-30_Human_Plasma__2_____xP1-_Inj 130  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DTXSID1024621-30_Human_Plasma_T0_1_____xP1-_Inj 131  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DTXSID1024621-30_Human_Plasma_T0_2_____xP1-_Inj 132  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DTXSID1024621-30_Human_PBS__1_____xP1-_Inj 127  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DTXSID1024621-30_Human_PBS__2_____xP1-_Inj 128  </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="10">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.000"/>
@@ -1115,18 +1113,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Normal 2" xfId="2"/>
-    <cellStyle name="Normal 3" xfId="3"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1158,7 +1156,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1446,10 +1450,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
@@ -1469,19 +1473,19 @@
       <c r="A1" s="68"/>
       <c r="B1" s="48"/>
       <c r="C1" s="67" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="68"/>
       <c r="B2" s="49"/>
       <c r="C2" s="67" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="66" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="C3" s="49">
         <v>44085.409236111111</v>
@@ -1489,36 +1493,36 @@
     </row>
     <row r="4" spans="1:8" s="51" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="52" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="B4" s="52" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="C4" s="52" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="D4" s="52" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="E4" s="52" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="F4" s="52" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="G4" s="52" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="H4" s="52" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A5" s="50" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C5" s="50">
         <v>5</v>
@@ -1526,18 +1530,18 @@
       <c r="D5" s="65">
         <v>10</v>
       </c>
-      <c r="E5" s="70" t="s">
-        <v>232</v>
-      </c>
-      <c r="F5" s="70"/>
-      <c r="G5" s="70"/>
+      <c r="E5" s="69" t="s">
+        <v>224</v>
+      </c>
+      <c r="F5" s="69"/>
+      <c r="G5" s="69"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="50" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C6" s="50">
         <v>5</v>
@@ -1545,16 +1549,16 @@
       <c r="D6" s="65">
         <v>100</v>
       </c>
-      <c r="E6" s="69"/>
-      <c r="F6" s="69"/>
-      <c r="G6" s="69"/>
+      <c r="E6" s="70"/>
+      <c r="F6" s="70"/>
+      <c r="G6" s="70"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="50" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="B7" s="50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C7" s="50">
         <v>5</v>
@@ -1562,16 +1566,16 @@
       <c r="D7" s="65">
         <v>30</v>
       </c>
-      <c r="E7" s="69"/>
-      <c r="F7" s="69"/>
-      <c r="G7" s="69"/>
+      <c r="E7" s="70"/>
+      <c r="F7" s="70"/>
+      <c r="G7" s="70"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="50" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="B8" s="50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C8" s="50">
         <v>5</v>
@@ -1591,10 +1595,10 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="50" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="B9" s="50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C9" s="50">
         <v>5</v>
@@ -1603,10 +1607,10 @@
         <v>100</v>
       </c>
       <c r="E9" s="53" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="F9" s="54" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="G9" s="53">
         <v>1.0453178764518638</v>
@@ -1614,10 +1618,10 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="50" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="B10" s="50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C10" s="50">
         <v>5</v>
@@ -1637,10 +1641,10 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="50" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="B11" s="50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C11" s="50">
         <v>5</v>
@@ -1649,10 +1653,10 @@
         <v>10</v>
       </c>
       <c r="E11" s="53" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="F11" s="54" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="G11" s="53">
         <v>1.4981518290887279</v>
@@ -1660,10 +1664,10 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="50" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="B12" s="50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C12" s="50">
         <v>5</v>
@@ -1672,10 +1676,10 @@
         <v>100</v>
       </c>
       <c r="E12" s="53" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="F12" s="54" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="G12" s="53">
         <v>1.3443779135875455</v>
@@ -1683,10 +1687,10 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="50" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="B13" s="50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C13" s="50">
         <v>5</v>
@@ -1695,10 +1699,10 @@
         <v>30</v>
       </c>
       <c r="E13" s="53" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="F13" s="54" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="G13" s="53">
         <v>1.628610244569578</v>
@@ -1706,10 +1710,10 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="50" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="B14" s="50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C14" s="50">
         <v>5</v>
@@ -1729,10 +1733,10 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="50" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="B15" s="50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C15" s="50">
         <v>5</v>
@@ -1752,10 +1756,10 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="50" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="B16" s="50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C16" s="50">
         <v>5</v>
@@ -1775,10 +1779,10 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="50" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="B17" s="50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C17" s="50">
         <v>5</v>
@@ -1798,10 +1802,10 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="50" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="B18" s="50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C18" s="50">
         <v>5</v>
@@ -1821,10 +1825,10 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="50" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="B19" s="50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C19" s="50">
         <v>5</v>
@@ -1844,10 +1848,10 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="50" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="B20" s="50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C20" s="50">
         <v>5</v>
@@ -1867,10 +1871,10 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="50" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="B21" s="50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C21" s="50">
         <v>5</v>
@@ -1890,10 +1894,10 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="50" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="B22" s="50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C22" s="50">
         <v>5</v>
@@ -1913,10 +1917,10 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="50" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="B23" s="50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C23" s="50">
         <v>2</v>
@@ -1936,10 +1940,10 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="50" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="B24" s="50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C24" s="50">
         <v>2</v>
@@ -1959,10 +1963,10 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="50" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="B25" s="50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C25" s="50">
         <v>2</v>
@@ -1982,10 +1986,10 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="50" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="B26" s="50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C26" s="50">
         <v>2</v>
@@ -2005,10 +2009,10 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="50" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="B27" s="50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C27" s="50">
         <v>2</v>
@@ -2028,10 +2032,10 @@
     </row>
     <row r="28" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="58" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="B28" s="58" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C28" s="58">
         <v>2</v>
@@ -2054,34 +2058,34 @@
     <row r="31" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="1:8" s="51" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="52" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="B32" s="52" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="C32" s="52" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="D32" s="52"/>
       <c r="E32" s="52" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="F32" s="52" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="G32" s="52" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="H32" s="52" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A33" s="50" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="B33" s="50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C33" s="50">
         <v>5</v>
@@ -2090,20 +2094,20 @@
         <v>10</v>
       </c>
       <c r="E33" s="50" t="s">
-        <v>218</v>
-      </c>
-      <c r="F33" s="70" t="s">
-        <v>232</v>
-      </c>
-      <c r="G33" s="70"/>
-      <c r="H33" s="70"/>
+        <v>211</v>
+      </c>
+      <c r="F33" s="69" t="s">
+        <v>224</v>
+      </c>
+      <c r="G33" s="69"/>
+      <c r="H33" s="69"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="50" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="B34" s="50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C34" s="50">
         <v>5</v>
@@ -2112,18 +2116,18 @@
         <v>10</v>
       </c>
       <c r="E34" s="50" t="s">
-        <v>219</v>
-      </c>
-      <c r="F34" s="69"/>
-      <c r="G34" s="69"/>
-      <c r="H34" s="69"/>
+        <v>212</v>
+      </c>
+      <c r="F34" s="70"/>
+      <c r="G34" s="70"/>
+      <c r="H34" s="70"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="50" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="B35" s="50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C35" s="50">
         <v>5</v>
@@ -2132,18 +2136,18 @@
         <v>100</v>
       </c>
       <c r="E35" s="50" t="s">
-        <v>218</v>
-      </c>
-      <c r="F35" s="69"/>
-      <c r="G35" s="69"/>
-      <c r="H35" s="69"/>
+        <v>211</v>
+      </c>
+      <c r="F35" s="70"/>
+      <c r="G35" s="70"/>
+      <c r="H35" s="70"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="50" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="B36" s="50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C36" s="50">
         <v>5</v>
@@ -2152,18 +2156,18 @@
         <v>100</v>
       </c>
       <c r="E36" s="50" t="s">
-        <v>219</v>
-      </c>
-      <c r="F36" s="69"/>
-      <c r="G36" s="69"/>
-      <c r="H36" s="69"/>
+        <v>212</v>
+      </c>
+      <c r="F36" s="70"/>
+      <c r="G36" s="70"/>
+      <c r="H36" s="70"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="50" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="B37" s="50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C37" s="50">
         <v>5</v>
@@ -2172,18 +2176,18 @@
         <v>30</v>
       </c>
       <c r="E37" s="50" t="s">
-        <v>218</v>
-      </c>
-      <c r="F37" s="69"/>
-      <c r="G37" s="69"/>
-      <c r="H37" s="69"/>
+        <v>211</v>
+      </c>
+      <c r="F37" s="70"/>
+      <c r="G37" s="70"/>
+      <c r="H37" s="70"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="50" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="B38" s="50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C38" s="50">
         <v>5</v>
@@ -2192,18 +2196,18 @@
         <v>30</v>
       </c>
       <c r="E38" s="50" t="s">
-        <v>219</v>
-      </c>
-      <c r="F38" s="69"/>
-      <c r="G38" s="69"/>
-      <c r="H38" s="69"/>
+        <v>212</v>
+      </c>
+      <c r="F38" s="70"/>
+      <c r="G38" s="70"/>
+      <c r="H38" s="70"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="50" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="B39" s="50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C39" s="50">
         <v>5</v>
@@ -2212,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E39" s="50" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="F39" s="56">
         <v>0.88929524625537248</v>
@@ -2226,10 +2230,10 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="50" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="B40" s="50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C40" s="50">
         <v>5</v>
@@ -2238,7 +2242,7 @@
         <v>10</v>
       </c>
       <c r="E40" s="50" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="F40" s="56">
         <v>0.11070475374462752</v>
@@ -2252,10 +2256,10 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="50" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="B41" s="50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C41" s="50">
         <v>5</v>
@@ -2264,24 +2268,24 @@
         <v>100</v>
       </c>
       <c r="E41" s="50" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="F41" s="53" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="G41" s="53" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="H41" s="53" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="50" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="B42" s="50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C42" s="50">
         <v>5</v>
@@ -2290,24 +2294,24 @@
         <v>100</v>
       </c>
       <c r="E42" s="50" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="F42" s="54" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="G42" s="54" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="H42" s="54" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="50" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="B43" s="50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C43" s="50">
         <v>5</v>
@@ -2316,7 +2320,7 @@
         <v>30</v>
       </c>
       <c r="E43" s="50" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="F43" s="56">
         <v>0.95375922065945318</v>
@@ -2330,10 +2334,10 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="50" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="B44" s="50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C44" s="50">
         <v>5</v>
@@ -2342,7 +2346,7 @@
         <v>30</v>
       </c>
       <c r="E44" s="50" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="F44" s="54">
         <v>4.6240779340546823E-2</v>
@@ -2356,10 +2360,10 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="50" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="B45" s="50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C45" s="50">
         <v>5</v>
@@ -2368,24 +2372,24 @@
         <v>10</v>
       </c>
       <c r="E45" s="50" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="F45" s="53" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="G45" s="53" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="H45" s="53" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="50" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="B46" s="50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C46" s="50">
         <v>5</v>
@@ -2394,24 +2398,24 @@
         <v>10</v>
       </c>
       <c r="E46" s="50" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="F46" s="54" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="G46" s="54" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="H46" s="54" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="50" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="B47" s="50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C47" s="50">
         <v>5</v>
@@ -2420,24 +2424,24 @@
         <v>100</v>
       </c>
       <c r="E47" s="50" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="F47" s="53" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="G47" s="56">
         <v>0.80511659745552244</v>
       </c>
       <c r="H47" s="53" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="50" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="B48" s="50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C48" s="50">
         <v>5</v>
@@ -2446,24 +2450,24 @@
         <v>100</v>
       </c>
       <c r="E48" s="50" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="F48" s="54" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="G48" s="56">
         <v>0.19488340254447756</v>
       </c>
       <c r="H48" s="54" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="50" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="B49" s="50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C49" s="50">
         <v>5</v>
@@ -2472,24 +2476,24 @@
         <v>30</v>
       </c>
       <c r="E49" s="50" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="F49" s="53" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="G49" s="53" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="H49" s="53" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="50" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="B50" s="50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C50" s="50">
         <v>5</v>
@@ -2498,24 +2502,24 @@
         <v>30</v>
       </c>
       <c r="E50" s="50" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="F50" s="54" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="G50" s="54" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="H50" s="54" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="50" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="B51" s="50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C51" s="50">
         <v>5</v>
@@ -2524,7 +2528,7 @@
         <v>10</v>
       </c>
       <c r="E51" s="50" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="F51" s="54">
         <v>1.7330408264724095E-2</v>
@@ -2538,10 +2542,10 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="50" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="B52" s="50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C52" s="50">
         <v>5</v>
@@ -2550,7 +2554,7 @@
         <v>10</v>
       </c>
       <c r="E52" s="50" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="F52" s="56">
         <v>0.9826695917352759</v>
@@ -2564,10 +2568,10 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="50" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="B53" s="50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C53" s="50">
         <v>5</v>
@@ -2576,7 +2580,7 @@
         <v>100</v>
       </c>
       <c r="E53" s="50" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="F53" s="62">
         <v>6.8682379128166162E-5</v>
@@ -2590,10 +2594,10 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="50" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="B54" s="50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C54" s="50">
         <v>5</v>
@@ -2602,7 +2606,7 @@
         <v>100</v>
       </c>
       <c r="E54" s="50" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="F54" s="56">
         <v>0.99993131762087184</v>
@@ -2616,10 +2620,10 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="50" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="B55" s="50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C55" s="50">
         <v>5</v>
@@ -2628,7 +2632,7 @@
         <v>30</v>
       </c>
       <c r="E55" s="50" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="F55" s="54">
         <v>2.4186306474149974E-2</v>
@@ -2642,10 +2646,10 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="50" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="B56" s="50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C56" s="50">
         <v>5</v>
@@ -2654,7 +2658,7 @@
         <v>30</v>
       </c>
       <c r="E56" s="50" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="F56" s="56">
         <v>0.97581369352585001</v>
@@ -2668,10 +2672,10 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="50" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="B57" s="50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C57" s="50">
         <v>5</v>
@@ -2680,7 +2684,7 @@
         <v>10</v>
       </c>
       <c r="E57" s="50" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="F57" s="56">
         <v>0.22648969452200449</v>
@@ -2694,10 +2698,10 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="50" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="B58" s="50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C58" s="50">
         <v>5</v>
@@ -2706,7 +2710,7 @@
         <v>10</v>
       </c>
       <c r="E58" s="50" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="F58" s="56">
         <v>0.77351030547799549</v>
@@ -2720,10 +2724,10 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="50" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="B59" s="50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C59" s="50">
         <v>5</v>
@@ -2732,7 +2736,7 @@
         <v>100</v>
       </c>
       <c r="E59" s="50" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="F59" s="54">
         <v>2.4258563229817239E-2</v>
@@ -2746,10 +2750,10 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="50" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="B60" s="50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C60" s="50">
         <v>5</v>
@@ -2758,7 +2762,7 @@
         <v>100</v>
       </c>
       <c r="E60" s="50" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="F60" s="56">
         <v>0.97574143677018277</v>
@@ -2772,10 +2776,10 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="50" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="B61" s="50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C61" s="50">
         <v>5</v>
@@ -2784,7 +2788,7 @@
         <v>30</v>
       </c>
       <c r="E61" s="50" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="F61" s="54">
         <v>8.6809172508791152E-2</v>
@@ -2798,10 +2802,10 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="50" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="B62" s="50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C62" s="50">
         <v>5</v>
@@ -2810,7 +2814,7 @@
         <v>30</v>
       </c>
       <c r="E62" s="50" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="F62" s="56">
         <v>0.91319082749120883</v>
@@ -2824,10 +2828,10 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="50" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="B63" s="50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C63" s="50">
         <v>5</v>
@@ -2836,7 +2840,7 @@
         <v>10</v>
       </c>
       <c r="E63" s="50" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="F63" s="56">
         <v>0.77441773377781387</v>
@@ -2850,10 +2854,10 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="50" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="B64" s="50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C64" s="50">
         <v>5</v>
@@ -2862,7 +2866,7 @@
         <v>10</v>
       </c>
       <c r="E64" s="50" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="F64" s="56">
         <v>0.22558226622218613</v>
@@ -2876,10 +2880,10 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="50" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="B65" s="50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C65" s="50">
         <v>5</v>
@@ -2888,7 +2892,7 @@
         <v>100</v>
       </c>
       <c r="E65" s="50" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="F65" s="56">
         <v>0.5093442504798098</v>
@@ -2902,10 +2906,10 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="50" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="B66" s="50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C66" s="50">
         <v>5</v>
@@ -2914,7 +2918,7 @@
         <v>100</v>
       </c>
       <c r="E66" s="50" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="F66" s="56">
         <v>0.4906557495201902</v>
@@ -2928,10 +2932,10 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="50" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="B67" s="50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C67" s="50">
         <v>5</v>
@@ -2940,7 +2944,7 @@
         <v>30</v>
       </c>
       <c r="E67" s="50" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="F67" s="56">
         <v>0.81764532937983581</v>
@@ -2954,10 +2958,10 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="50" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="B68" s="50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C68" s="50">
         <v>5</v>
@@ -2966,7 +2970,7 @@
         <v>30</v>
       </c>
       <c r="E68" s="50" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="F68" s="56">
         <v>0.18235467062016419</v>
@@ -2980,10 +2984,10 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="50" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="B69" s="50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C69" s="50">
         <v>2</v>
@@ -2992,7 +2996,7 @@
         <v>10</v>
       </c>
       <c r="E69" s="50" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="F69" s="56">
         <v>0.77845754278862211</v>
@@ -3006,10 +3010,10 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="50" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="B70" s="50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C70" s="50">
         <v>2</v>
@@ -3018,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E70" s="50" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="F70" s="56">
         <v>0.22154245721137789</v>
@@ -3032,10 +3036,10 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="50" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="B71" s="50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C71" s="50">
         <v>2</v>
@@ -3044,7 +3048,7 @@
         <v>100</v>
       </c>
       <c r="E71" s="50" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="F71" s="56">
         <v>0.31258282260340198</v>
@@ -3058,10 +3062,10 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="50" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="B72" s="50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C72" s="50">
         <v>2</v>
@@ -3070,7 +3074,7 @@
         <v>100</v>
       </c>
       <c r="E72" s="50" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="F72" s="56">
         <v>0.68741717739659802</v>
@@ -3084,10 +3088,10 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="50" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="B73" s="50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C73" s="50">
         <v>2</v>
@@ -3096,7 +3100,7 @@
         <v>30</v>
       </c>
       <c r="E73" s="50" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="F73" s="56">
         <v>0.62575316535115666</v>
@@ -3110,10 +3114,10 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="50" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="B74" s="50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C74" s="50">
         <v>2</v>
@@ -3122,7 +3126,7 @@
         <v>30</v>
       </c>
       <c r="E74" s="50" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="F74" s="56">
         <v>0.37424683464884334</v>
@@ -3136,10 +3140,10 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="50" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="B75" s="50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C75" s="50">
         <v>2</v>
@@ -3148,7 +3152,7 @@
         <v>10</v>
       </c>
       <c r="E75" s="50" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="F75" s="54">
         <v>8.5374929724691753E-2</v>
@@ -3162,10 +3166,10 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="50" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="B76" s="50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C76" s="50">
         <v>2</v>
@@ -3174,7 +3178,7 @@
         <v>10</v>
       </c>
       <c r="E76" s="50" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="F76" s="56">
         <v>0.91462507027530826</v>
@@ -3188,10 +3192,10 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="50" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="B77" s="50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C77" s="50">
         <v>2</v>
@@ -3200,7 +3204,7 @@
         <v>100</v>
       </c>
       <c r="E77" s="50" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="F77" s="55">
         <v>6.9294810832601318E-3</v>
@@ -3214,10 +3218,10 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="50" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="B78" s="50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C78" s="50">
         <v>2</v>
@@ -3226,7 +3230,7 @@
         <v>100</v>
       </c>
       <c r="E78" s="50" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="F78" s="56">
         <v>0.99307051891673992</v>
@@ -3240,10 +3244,10 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="50" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="B79" s="50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C79" s="50">
         <v>2</v>
@@ -3252,7 +3256,7 @@
         <v>30</v>
       </c>
       <c r="E79" s="50" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="F79" s="54">
         <v>2.3088097222424941E-2</v>
@@ -3266,10 +3270,10 @@
     </row>
     <row r="80" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="58" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="B80" s="58" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C80" s="58">
         <v>2</v>
@@ -3278,7 +3282,7 @@
         <v>30</v>
       </c>
       <c r="E80" s="58" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="F80" s="60">
         <v>0.976911902777575</v>
@@ -3304,11 +3308,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K216"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="M37" sqref="M37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3347,19 +3351,19 @@
         <v>5</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -3382,7 +3386,7 @@
         <v>1.885E-7</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -3405,13 +3409,13 @@
         <v>2.4572E-6</v>
       </c>
       <c r="H3" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="I3" s="6">
         <v>1.32285E-6</v>
       </c>
       <c r="J3" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -3507,7 +3511,7 @@
         <v>1.7724005382500003</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="I6" s="12">
         <v>4.7602794028068391</v>
@@ -3601,7 +3605,7 @@
         <v>36</v>
       </c>
       <c r="B11" s="47" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="C11" s="47" t="s">
         <v>38</v>
@@ -3616,7 +3620,7 @@
         <v>2.0989999999999999E-7</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -3624,7 +3628,7 @@
         <v>39</v>
       </c>
       <c r="B12" s="46" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="C12" s="46" t="s">
         <v>38</v>
@@ -3639,21 +3643,21 @@
         <v>2.195E-7</v>
       </c>
       <c r="H12" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="I12" s="6">
         <v>2.1469999999999998E-7</v>
       </c>
       <c r="J12" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="47" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="B13" s="47" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="C13" s="47" t="s">
         <v>38</v>
@@ -3685,10 +3689,10 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="46" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="B14" s="46" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="C14" s="46" t="s">
         <v>38</v>
@@ -3720,10 +3724,10 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="47" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="B15" s="47" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="C15" s="47" t="s">
         <v>38</v>
@@ -3741,7 +3745,7 @@
         <v>0.11271215449999999</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="I15" s="12">
         <v>5.0783646701006981</v>
@@ -3755,10 +3759,10 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="46" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="B16" s="46" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="C16" s="46" t="s">
         <v>38</v>
@@ -3778,10 +3782,10 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="47" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="B17" s="47" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="C17" s="47" t="s">
         <v>38</v>
@@ -3801,10 +3805,10 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="46" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="B18" s="46" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="C18" s="46" t="s">
         <v>38</v>
@@ -3850,7 +3854,7 @@
         <v>1.0860000000000001E-7</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -3873,13 +3877,13 @@
         <v>4.0349999999999998E-7</v>
       </c>
       <c r="H21" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="I21" s="6">
         <v>2.5604999999999997E-7</v>
       </c>
       <c r="J21" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -3975,7 +3979,7 @@
         <v>1.0785002407499999</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="I24" s="12">
         <v>24.818505831127677</v>
@@ -4084,7 +4088,7 @@
         <v>6.1944999999999997E-6</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -4107,13 +4111,13 @@
         <v>9.4307999999999996E-6</v>
       </c>
       <c r="H30" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="I30" s="6">
         <v>7.8126500000000005E-6</v>
       </c>
       <c r="J30" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -4209,7 +4213,7 @@
         <v>0.60965173075000001</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="I33" s="28">
         <v>0.98239942095028321</v>
@@ -4303,7 +4307,7 @@
         <v>56</v>
       </c>
       <c r="B38" s="46" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="C38" s="46" t="s">
         <v>58</v>
@@ -4318,7 +4322,7 @@
         <v>1.7380999999999998E-5</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
@@ -4326,7 +4330,7 @@
         <v>59</v>
       </c>
       <c r="B39" s="47" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="C39" s="47" t="s">
         <v>58</v>
@@ -4341,21 +4345,21 @@
         <v>9.329E-6</v>
       </c>
       <c r="H39" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="I39" s="6">
         <v>1.3355E-5</v>
       </c>
       <c r="J39" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="46" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="B40" s="46" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="C40" s="46" t="s">
         <v>58</v>
@@ -4387,10 +4391,10 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="47" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="B41" s="47" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="C41" s="47" t="s">
         <v>58</v>
@@ -4422,10 +4426,10 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="46" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="B42" s="46" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="C42" s="46" t="s">
         <v>58</v>
@@ -4443,7 +4447,7 @@
         <v>0.61388259199999995</v>
       </c>
       <c r="H42" s="5" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="I42" s="12">
         <v>1.0636366918096365</v>
@@ -4457,10 +4461,10 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="47" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="B43" s="47" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="C43" s="47" t="s">
         <v>58</v>
@@ -4480,10 +4484,10 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="46" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="B44" s="46" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="C44" s="46" t="s">
         <v>58</v>
@@ -4503,10 +4507,10 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="47" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="B45" s="47" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="C45" s="47" t="s">
         <v>58</v>
@@ -4537,7 +4541,7 @@
         <v>56</v>
       </c>
       <c r="B47" s="47" t="s">
-        <v>121</v>
+        <v>227</v>
       </c>
       <c r="C47" s="47" t="s">
         <v>58</v>
@@ -4552,7 +4556,7 @@
         <v>3.8083999999999998E-6</v>
       </c>
       <c r="I47" s="3" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
@@ -4560,7 +4564,7 @@
         <v>59</v>
       </c>
       <c r="B48" s="46" t="s">
-        <v>121</v>
+        <v>227</v>
       </c>
       <c r="C48" s="46" t="s">
         <v>58</v>
@@ -4575,21 +4579,21 @@
         <v>2.4901200000000001E-5</v>
       </c>
       <c r="H48" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="I48" s="6">
         <v>1.43548E-5</v>
       </c>
       <c r="J48" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="47" t="s">
-        <v>124</v>
+        <v>228</v>
       </c>
       <c r="B49" s="47" t="s">
-        <v>121</v>
+        <v>227</v>
       </c>
       <c r="C49" s="47" t="s">
         <v>58</v>
@@ -4621,10 +4625,10 @@
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="46" t="s">
-        <v>125</v>
+        <v>229</v>
       </c>
       <c r="B50" s="46" t="s">
-        <v>121</v>
+        <v>227</v>
       </c>
       <c r="C50" s="46" t="s">
         <v>58</v>
@@ -4656,10 +4660,10 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="47" t="s">
-        <v>126</v>
+        <v>230</v>
       </c>
       <c r="B51" s="47" t="s">
-        <v>121</v>
+        <v>227</v>
       </c>
       <c r="C51" s="47" t="s">
         <v>58</v>
@@ -4677,7 +4681,7 @@
         <v>0.65544252999999997</v>
       </c>
       <c r="H51" s="5" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="I51" s="28">
         <v>0.95098820755569224</v>
@@ -4691,10 +4695,10 @@
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="46" t="s">
-        <v>127</v>
+        <v>231</v>
       </c>
       <c r="B52" s="46" t="s">
-        <v>121</v>
+        <v>227</v>
       </c>
       <c r="C52" s="46" t="s">
         <v>58</v>
@@ -4714,10 +4718,10 @@
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="47" t="s">
-        <v>122</v>
+        <v>232</v>
       </c>
       <c r="B53" s="47" t="s">
-        <v>121</v>
+        <v>227</v>
       </c>
       <c r="C53" s="47" t="s">
         <v>58</v>
@@ -4737,10 +4741,10 @@
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="46" t="s">
-        <v>123</v>
+        <v>233</v>
       </c>
       <c r="B54" s="46" t="s">
-        <v>121</v>
+        <v>227</v>
       </c>
       <c r="C54" s="46" t="s">
         <v>58</v>
@@ -4786,7 +4790,7 @@
         <v>-9.5000000000000007E-9</v>
       </c>
       <c r="I56" s="3" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
@@ -4809,13 +4813,13 @@
         <v>4.2371999999999999E-6</v>
       </c>
       <c r="H57" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="I57" s="6">
         <v>2.1138500000000001E-6</v>
       </c>
       <c r="J57" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
@@ -4911,7 +4915,7 @@
         <v>5.5854225749999993E-2</v>
       </c>
       <c r="H60" s="5" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="I60" s="12">
         <v>1.06562718319327</v>
@@ -5005,7 +5009,7 @@
         <v>76</v>
       </c>
       <c r="B65" s="47" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="C65" s="47" t="s">
         <v>78</v>
@@ -5020,7 +5024,7 @@
         <v>2.84376E-5</v>
       </c>
       <c r="I65" s="3" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
@@ -5028,7 +5032,7 @@
         <v>79</v>
       </c>
       <c r="B66" s="46" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="C66" s="46" t="s">
         <v>78</v>
@@ -5043,21 +5047,21 @@
         <v>1.237E-7</v>
       </c>
       <c r="H66" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="I66" s="6">
         <v>1.428065E-5</v>
       </c>
       <c r="J66" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="47" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="B67" s="47" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="C67" s="47" t="s">
         <v>78</v>
@@ -5089,10 +5093,10 @@
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="46" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="B68" s="46" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="C68" s="46" t="s">
         <v>78</v>
@@ -5124,10 +5128,10 @@
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="47" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="B69" s="47" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="C69" s="47" t="s">
         <v>78</v>
@@ -5145,7 +5149,7 @@
         <v>5.6690636749999995E-2</v>
       </c>
       <c r="H69" s="5" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="I69" s="12">
         <v>1.1444184358269565</v>
@@ -5159,10 +5163,10 @@
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="46" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="B70" s="46" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="C70" s="46" t="s">
         <v>78</v>
@@ -5182,10 +5186,10 @@
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="47" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="B71" s="47" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="C71" s="47" t="s">
         <v>78</v>
@@ -5205,10 +5209,10 @@
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="46" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="B72" s="46" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="C72" s="46" t="s">
         <v>78</v>
@@ -5239,7 +5243,7 @@
         <v>76</v>
       </c>
       <c r="B74" s="46" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="C74" s="46" t="s">
         <v>78</v>
@@ -5254,7 +5258,7 @@
         <v>2.1835400000000001E-5</v>
       </c>
       <c r="I74" s="3" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
@@ -5262,7 +5266,7 @@
         <v>79</v>
       </c>
       <c r="B75" s="47" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="C75" s="47" t="s">
         <v>78</v>
@@ -5277,21 +5281,21 @@
         <v>9.3379999999999996E-7</v>
       </c>
       <c r="H75" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="I75" s="6">
         <v>1.1384600000000001E-5</v>
       </c>
       <c r="J75" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="46" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="B76" s="46" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="C76" s="46" t="s">
         <v>78</v>
@@ -5323,10 +5327,10 @@
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="47" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="B77" s="47" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="C77" s="47" t="s">
         <v>78</v>
@@ -5358,10 +5362,10 @@
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="46" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="B78" s="46" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="C78" s="46" t="s">
         <v>78</v>
@@ -5379,7 +5383,7 @@
         <v>6.7258241499999996E-2</v>
       </c>
       <c r="H78" s="5" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="I78" s="12">
         <v>1.3278579057182089</v>
@@ -5393,10 +5397,10 @@
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="47" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="B79" s="47" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="C79" s="47" t="s">
         <v>78</v>
@@ -5416,10 +5420,10 @@
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="46" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="B80" s="46" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="C80" s="46" t="s">
         <v>78</v>
@@ -5439,10 +5443,10 @@
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="47" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="B81" s="47" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="C81" s="47" t="s">
         <v>78</v>
@@ -5488,7 +5492,7 @@
         <v>1.4360000000000001E-6</v>
       </c>
       <c r="I83" s="3" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
@@ -5511,13 +5515,13 @@
         <v>4.8902000000000002E-6</v>
       </c>
       <c r="H84" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="I84" s="6">
         <v>3.1631000000000003E-6</v>
       </c>
       <c r="J84" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
@@ -5613,7 +5617,7 @@
         <v>0.16928725</v>
       </c>
       <c r="H87" s="5" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="I87" s="39">
         <v>2.2144592318979868E-2</v>
@@ -5707,7 +5711,7 @@
         <v>26</v>
       </c>
       <c r="B92" s="46" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="C92" s="46" t="s">
         <v>28</v>
@@ -5722,7 +5726,7 @@
         <v>2.4783999999999999E-6</v>
       </c>
       <c r="I92" s="3" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
@@ -5730,7 +5734,7 @@
         <v>29</v>
       </c>
       <c r="B93" s="47" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="C93" s="47" t="s">
         <v>28</v>
@@ -5745,21 +5749,21 @@
         <v>8.65E-8</v>
       </c>
       <c r="H93" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="I93" s="6">
         <v>1.2824499999999999E-6</v>
       </c>
       <c r="J93" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="46" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="B94" s="46" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="C94" s="46" t="s">
         <v>28</v>
@@ -5791,10 +5795,10 @@
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="47" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="B95" s="47" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="C95" s="47" t="s">
         <v>28</v>
@@ -5826,10 +5830,10 @@
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="46" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="B96" s="46" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="C96" s="46" t="s">
         <v>28</v>
@@ -5847,7 +5851,7 @@
         <v>0.44803661475000001</v>
       </c>
       <c r="H96" s="5" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="I96" s="42">
         <v>1.2393129147310664E-4</v>
@@ -5861,10 +5865,10 @@
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="47" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="B97" s="47" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="C97" s="47" t="s">
         <v>28</v>
@@ -5884,10 +5888,10 @@
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="46" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B98" s="46" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="C98" s="46" t="s">
         <v>28</v>
@@ -5907,10 +5911,10 @@
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="47" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="B99" s="47" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="C99" s="47" t="s">
         <v>28</v>
@@ -5956,7 +5960,7 @@
         <v>4.5434900000000001E-5</v>
       </c>
       <c r="I101" s="3" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.25">
@@ -5979,13 +5983,13 @@
         <v>1.511E-7</v>
       </c>
       <c r="H102" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="I102" s="6">
         <v>2.2793E-5</v>
       </c>
       <c r="J102" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.25">
@@ -6081,7 +6085,7 @@
         <v>0.105502253</v>
       </c>
       <c r="H105" s="5" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="I105" s="39">
         <v>1.9449326431648237E-2</v>
@@ -6190,7 +6194,7 @@
         <v>8.5531436999999998E-3</v>
       </c>
       <c r="I110" s="3" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.25">
@@ -6213,13 +6217,13 @@
         <v>1.0343271100000001E-2</v>
       </c>
       <c r="H111" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="I111" s="20">
         <v>9.4482074000000003E-3</v>
       </c>
       <c r="J111" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.25">
@@ -6315,7 +6319,7 @@
         <v>4.4027968655</v>
       </c>
       <c r="H114" s="5" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="I114" s="28">
         <v>0.22457026800691476</v>
@@ -6409,7 +6413,7 @@
         <v>46</v>
       </c>
       <c r="B119" s="47" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="C119" s="47" t="s">
         <v>48</v>
@@ -6424,7 +6428,7 @@
         <v>1.9798490000000001E-3</v>
       </c>
       <c r="I119" s="3" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
     </row>
     <row r="120" spans="1:11" x14ac:dyDescent="0.25">
@@ -6432,7 +6436,7 @@
         <v>49</v>
       </c>
       <c r="B120" s="46" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="C120" s="46" t="s">
         <v>48</v>
@@ -6447,21 +6451,21 @@
         <v>3.1508324999999998E-3</v>
       </c>
       <c r="H120" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="I120" s="20">
         <v>2.5653407499999998E-3</v>
       </c>
       <c r="J120" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
     </row>
     <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121" s="47" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="B121" s="47" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="C121" s="47" t="s">
         <v>48</v>
@@ -6493,10 +6497,10 @@
     </row>
     <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" s="46" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="B122" s="46" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="C122" s="46" t="s">
         <v>48</v>
@@ -6528,10 +6532,10 @@
     </row>
     <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" s="47" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="B123" s="47" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="C123" s="47" t="s">
         <v>48</v>
@@ -6549,7 +6553,7 @@
         <v>2.8087673682499998</v>
       </c>
       <c r="H123" s="5" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="I123" s="39">
         <v>2.5867610480862654E-2</v>
@@ -6563,10 +6567,10 @@
     </row>
     <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124" s="46" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="B124" s="46" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="C124" s="46" t="s">
         <v>48</v>
@@ -6586,10 +6590,10 @@
     </row>
     <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125" s="47" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="B125" s="47" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="C125" s="47" t="s">
         <v>48</v>
@@ -6609,10 +6613,10 @@
     </row>
     <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126" s="46" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="B126" s="46" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="C126" s="46" t="s">
         <v>48</v>
@@ -6658,7 +6662,7 @@
         <v>6.7218360999999997E-3</v>
       </c>
       <c r="I128" s="3" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
     </row>
     <row r="129" spans="1:11" x14ac:dyDescent="0.25">
@@ -6681,13 +6685,13 @@
         <v>3.3351542E-3</v>
       </c>
       <c r="H129" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="I129" s="20">
         <v>5.0284951499999994E-3</v>
       </c>
       <c r="J129" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
     </row>
     <row r="130" spans="1:11" x14ac:dyDescent="0.25">
@@ -6783,7 +6787,7 @@
         <v>3.3126558242499997</v>
       </c>
       <c r="H132" s="5" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="I132" s="39">
         <v>8.8694264543044327E-2</v>
@@ -6892,7 +6896,7 @@
         <v>7.1018000000000003E-6</v>
       </c>
       <c r="I137" s="3" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
     </row>
     <row r="138" spans="1:11" x14ac:dyDescent="0.25">
@@ -6915,13 +6919,13 @@
         <v>2.616141E-4</v>
       </c>
       <c r="H138" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="I138" s="25">
         <v>1.3435794999999999E-4</v>
       </c>
       <c r="J138" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
     </row>
     <row r="139" spans="1:11" x14ac:dyDescent="0.25">
@@ -7017,7 +7021,7 @@
         <v>2.3129886749999995E-2</v>
       </c>
       <c r="H141" s="5" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="I141" s="28">
         <v>0.64845314828849632</v>
@@ -7111,7 +7115,7 @@
         <v>66</v>
       </c>
       <c r="B146" s="46" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="C146" s="46" t="s">
         <v>68</v>
@@ -7126,7 +7130,7 @@
         <v>3.4129E-6</v>
       </c>
       <c r="I146" s="3" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
     </row>
     <row r="147" spans="1:11" x14ac:dyDescent="0.25">
@@ -7134,7 +7138,7 @@
         <v>69</v>
       </c>
       <c r="B147" s="47" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="C147" s="47" t="s">
         <v>68</v>
@@ -7149,21 +7153,21 @@
         <v>4.5430000000000004E-6</v>
       </c>
       <c r="H147" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="I147" s="6">
         <v>3.9779499999999998E-6</v>
       </c>
       <c r="J147" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
     </row>
     <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A148" s="46" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="B148" s="46" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="C148" s="46" t="s">
         <v>68</v>
@@ -7195,10 +7199,10 @@
     </row>
     <row r="149" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A149" s="47" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="B149" s="47" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="C149" s="47" t="s">
         <v>68</v>
@@ -7230,10 +7234,10 @@
     </row>
     <row r="150" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A150" s="46" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="B150" s="46" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="C150" s="46" t="s">
         <v>68</v>
@@ -7251,7 +7255,7 @@
         <v>2.0102846887160492E-2</v>
       </c>
       <c r="H150" s="5" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="I150" s="28">
         <v>0.60221421077866988</v>
@@ -7265,10 +7269,10 @@
     </row>
     <row r="151" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A151" s="47" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="B151" s="47" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="C151" s="47" t="s">
         <v>68</v>
@@ -7288,10 +7292,10 @@
     </row>
     <row r="152" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A152" s="46" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="B152" s="46" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="C152" s="46" t="s">
         <v>68</v>
@@ -7311,10 +7315,10 @@
     </row>
     <row r="153" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A153" s="47" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="B153" s="47" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="C153" s="47" t="s">
         <v>68</v>
@@ -7345,7 +7349,7 @@
         <v>66</v>
       </c>
       <c r="B155" s="47" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="C155" s="47" t="s">
         <v>68</v>
@@ -7360,7 +7364,7 @@
         <v>3.9758000000000001E-6</v>
       </c>
       <c r="I155" s="3" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
     </row>
     <row r="156" spans="1:11" x14ac:dyDescent="0.25">
@@ -7368,7 +7372,7 @@
         <v>69</v>
       </c>
       <c r="B156" s="46" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="C156" s="46" t="s">
         <v>68</v>
@@ -7383,21 +7387,21 @@
         <v>1.13123E-5</v>
       </c>
       <c r="H156" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="I156" s="6">
         <v>7.6440500000000001E-6</v>
       </c>
       <c r="J156" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
     </row>
     <row r="157" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A157" s="47" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="B157" s="47" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="C157" s="47" t="s">
         <v>68</v>
@@ -7429,10 +7433,10 @@
     </row>
     <row r="158" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A158" s="46" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="B158" s="46" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="C158" s="46" t="s">
         <v>68</v>
@@ -7464,10 +7468,10 @@
     </row>
     <row r="159" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A159" s="47" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="B159" s="47" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="C159" s="47" t="s">
         <v>68</v>
@@ -7485,7 +7489,7 @@
         <v>2.3690398749999998E-2</v>
       </c>
       <c r="H159" s="5" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="I159" s="28">
         <v>0.73899881686289182</v>
@@ -7499,10 +7503,10 @@
     </row>
     <row r="160" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A160" s="46" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="B160" s="46" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="C160" s="46" t="s">
         <v>68</v>
@@ -7522,10 +7526,10 @@
     </row>
     <row r="161" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A161" s="47" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="B161" s="47" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="C161" s="47" t="s">
         <v>68</v>
@@ -7545,10 +7549,10 @@
     </row>
     <row r="162" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A162" s="46" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="B162" s="46" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="C162" s="46" t="s">
         <v>68</v>
@@ -7594,7 +7598,7 @@
         <v>8.2040000000000001E-7</v>
       </c>
       <c r="I164" s="3" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
     </row>
     <row r="165" spans="1:11" x14ac:dyDescent="0.25">
@@ -7617,13 +7621,13 @@
         <v>5.5907999999999999E-6</v>
       </c>
       <c r="H165" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="I165" s="6">
         <v>3.2055999999999999E-6</v>
       </c>
       <c r="J165" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
     </row>
     <row r="166" spans="1:11" x14ac:dyDescent="0.25">
@@ -7719,7 +7723,7 @@
         <v>1.1652651064999999</v>
       </c>
       <c r="H168" s="5" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="I168" s="28">
         <v>0.75708284230975442</v>
@@ -7813,7 +7817,7 @@
         <v>6</v>
       </c>
       <c r="B173" s="46" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C173" s="46" t="s">
         <v>8</v>
@@ -7828,7 +7832,7 @@
         <v>1.99E-7</v>
       </c>
       <c r="I173" s="3" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
     </row>
     <row r="174" spans="1:11" x14ac:dyDescent="0.25">
@@ -7836,7 +7840,7 @@
         <v>9</v>
       </c>
       <c r="B174" s="47" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C174" s="47" t="s">
         <v>8</v>
@@ -7851,21 +7855,21 @@
         <v>1.7839899999999998E-5</v>
       </c>
       <c r="H174" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="I174" s="6">
         <v>9.0194499999999988E-6</v>
       </c>
       <c r="J174" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
     </row>
     <row r="175" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A175" s="46" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="B175" s="46" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C175" s="46" t="s">
         <v>8</v>
@@ -7897,10 +7901,10 @@
     </row>
     <row r="176" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A176" s="47" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="B176" s="47" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C176" s="47" t="s">
         <v>8</v>
@@ -7932,10 +7936,10 @@
     </row>
     <row r="177" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A177" s="46" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="B177" s="46" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C177" s="46" t="s">
         <v>8</v>
@@ -7953,7 +7957,7 @@
         <v>1.4034097777500001</v>
       </c>
       <c r="H177" s="5" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="I177" s="28">
         <v>0.31924899957521491</v>
@@ -7967,10 +7971,10 @@
     </row>
     <row r="178" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A178" s="47" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="B178" s="47" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C178" s="47" t="s">
         <v>8</v>
@@ -7990,10 +7994,10 @@
     </row>
     <row r="179" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A179" s="46" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B179" s="46" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C179" s="46" t="s">
         <v>8</v>
@@ -8013,10 +8017,10 @@
     </row>
     <row r="180" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A180" s="47" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="B180" s="47" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C180" s="47" t="s">
         <v>8</v>
@@ -8062,7 +8066,7 @@
         <v>3.8451093961307984E-6</v>
       </c>
       <c r="I182" s="3" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
     </row>
     <row r="183" spans="1:11" x14ac:dyDescent="0.25">
@@ -8085,13 +8089,13 @@
         <v>2.4169999999999999E-6</v>
       </c>
       <c r="H183" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="I183" s="6">
         <v>3.1310546980653992E-6</v>
       </c>
       <c r="J183" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
     </row>
     <row r="184" spans="1:11" x14ac:dyDescent="0.25">
@@ -8187,7 +8191,7 @@
         <v>1.2638917732265096</v>
       </c>
       <c r="H186" s="5" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="I186" s="28">
         <v>0.56821869918173262</v>
@@ -8296,7 +8300,7 @@
         <v>4.0886400000000002E-5</v>
       </c>
       <c r="I191" s="3" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
     </row>
     <row r="192" spans="1:11" x14ac:dyDescent="0.25">
@@ -8319,13 +8323,13 @@
         <v>2.2797E-6</v>
       </c>
       <c r="H192" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="I192" s="6">
         <v>2.158305E-5</v>
       </c>
       <c r="J192" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
     </row>
     <row r="193" spans="1:11" x14ac:dyDescent="0.25">
@@ -8421,7 +8425,7 @@
         <v>0.28781751124999999</v>
       </c>
       <c r="H195" s="5" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="I195" s="39">
         <v>7.9946772755989243E-2</v>
@@ -8515,7 +8519,7 @@
         <v>16</v>
       </c>
       <c r="B200" s="47" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="C200" s="47" t="s">
         <v>18</v>
@@ -8530,7 +8534,7 @@
         <v>6.807E-7</v>
       </c>
       <c r="I200" s="3" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
     </row>
     <row r="201" spans="1:11" x14ac:dyDescent="0.25">
@@ -8538,7 +8542,7 @@
         <v>19</v>
       </c>
       <c r="B201" s="46" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="C201" s="46" t="s">
         <v>18</v>
@@ -8553,21 +8557,21 @@
         <v>2.0864E-6</v>
       </c>
       <c r="H201" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="I201" s="6">
         <v>1.3835500000000001E-6</v>
       </c>
       <c r="J201" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
     </row>
     <row r="202" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A202" s="47" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="B202" s="47" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="C202" s="47" t="s">
         <v>18</v>
@@ -8599,10 +8603,10 @@
     </row>
     <row r="203" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A203" s="46" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="B203" s="46" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="C203" s="46" t="s">
         <v>18</v>
@@ -8634,10 +8638,10 @@
     </row>
     <row r="204" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A204" s="47" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="B204" s="47" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="C204" s="47" t="s">
         <v>18</v>
@@ -8655,7 +8659,7 @@
         <v>0.27947474475</v>
       </c>
       <c r="H204" s="5" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="I204" s="45">
         <v>7.12747717785481E-3</v>
@@ -8669,10 +8673,10 @@
     </row>
     <row r="205" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A205" s="46" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="B205" s="46" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="C205" s="46" t="s">
         <v>18</v>
@@ -8692,10 +8696,10 @@
     </row>
     <row r="206" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A206" s="47" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="B206" s="47" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="C206" s="47" t="s">
         <v>18</v>
@@ -8715,10 +8719,10 @@
     </row>
     <row r="207" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A207" s="46" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="B207" s="46" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="C207" s="46" t="s">
         <v>18</v>
@@ -8764,7 +8768,7 @@
         <v>6.3507899999999995E-5</v>
       </c>
       <c r="I209" s="3" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
     </row>
     <row r="210" spans="1:11" x14ac:dyDescent="0.25">
@@ -8787,13 +8791,13 @@
         <v>8.2859999999999999E-7</v>
       </c>
       <c r="H210" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="I210" s="6">
         <v>3.2168249999999998E-5</v>
       </c>
       <c r="J210" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
     </row>
     <row r="211" spans="1:11" x14ac:dyDescent="0.25">
@@ -8889,7 +8893,7 @@
         <v>0.22276473975</v>
       </c>
       <c r="H213" s="5" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="I213" s="39">
         <v>2.3762490191784495E-2</v>

</xml_diff>